<commit_message>
se crea nuevo libro y se coloca los encabezados
</commit_message>
<xml_diff>
--- a/Insumo.xlsx
+++ b/Insumo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Diana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092051E4-D8FB-41B2-A545-B0BBB3911184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE958B3E-A588-4419-9665-F282FC083CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1529,9 +1529,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P214"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="4" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>